<commit_message>
FCDO core contribution projects added
</commit_message>
<xml_diff>
--- a/Inputs/MODARI award data - GHS (GAMRIF and UKVN).xlsx
+++ b/Inputs/MODARI award data - GHS (GAMRIF and UKVN).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{E4CC7446-E93A-46D5-86D9-2234D76FE536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6A1BF6D-4F29-4017-826E-8D4062A138E8}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{E4CC7446-E93A-46D5-86D9-2234D76FE536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F070C54-00FB-4B0F-8A2C-00D5A8055DA6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry sheet" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -988,10 +987,6 @@
     <t>https://d-portal.org/ctrack.html#view=act&amp;aid=XM-DAC-301-2-109057-001</t>
   </si>
   <si>
-    <t xml:space="preserve">GB-GOV-10-GAMRIF-WP5-FIND
-</t>
-  </si>
-  <si>
     <t>Foundation for New innovative Diagnostics</t>
   </si>
   <si>
@@ -2342,6 +2337,9 @@
   </si>
   <si>
     <t>Vaccine Efficacy Evaluation for Priority Emerging Diseases (VEEPED)</t>
+  </si>
+  <si>
+    <t>GB-GOV-10-GAMRIF-WP5-FIND</t>
   </si>
 </sst>
 </file>
@@ -2845,7 +2843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X988"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -4704,19 +4704,19 @@
         <v>61</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="G33" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="22">
@@ -4732,10 +4732,10 @@
         <v>5120528</v>
       </c>
       <c r="N33" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="O33" s="27" t="s">
         <v>273</v>
-      </c>
-      <c r="O33" s="27" t="s">
-        <v>274</v>
       </c>
       <c r="P33" s="33" t="s">
         <v>178</v>
@@ -4756,19 +4756,19 @@
         <v>61</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="F34" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="22">
@@ -4784,10 +4784,10 @@
         <v>4999705</v>
       </c>
       <c r="N34" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="O34" s="27" t="s">
         <v>273</v>
-      </c>
-      <c r="O34" s="27" t="s">
-        <v>274</v>
       </c>
       <c r="P34" s="33" t="s">
         <v>178</v>
@@ -4808,19 +4808,19 @@
         <v>61</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E35" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="F35" s="26" t="s">
         <v>279</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="G35" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="34" t="s">
         <v>281</v>
-      </c>
-      <c r="H35" s="34" t="s">
-        <v>282</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="22">
@@ -4836,10 +4836,10 @@
         <v>1000000</v>
       </c>
       <c r="N35" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O35" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P35" s="33" t="s">
         <v>178</v>
@@ -4860,19 +4860,19 @@
         <v>61</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E36" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E36" s="27" t="s">
-        <v>279</v>
-      </c>
       <c r="F36" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G36" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="H36" s="34" t="s">
         <v>281</v>
-      </c>
-      <c r="H36" s="34" t="s">
-        <v>282</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="22">
@@ -4888,10 +4888,10 @@
         <v>5000000</v>
       </c>
       <c r="N36" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O36" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P36" s="33" t="s">
         <v>178</v>
@@ -4912,19 +4912,19 @@
         <v>61</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E37" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E37" s="27" t="s">
-        <v>279</v>
-      </c>
       <c r="F37" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="22">
@@ -4940,10 +4940,10 @@
         <v>1000000</v>
       </c>
       <c r="N37" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O37" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P37" s="33" t="s">
         <v>178</v>
@@ -4964,19 +4964,19 @@
         <v>61</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="G38" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="G38" s="38" t="s">
+      <c r="H38" s="25" t="s">
         <v>290</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>291</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="22">
@@ -4995,13 +4995,13 @@
         <v>257</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P38" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="R38" s="2" t="s">
         <v>257</v>
@@ -5022,19 +5022,19 @@
         <v>61</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F39" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="25" t="s">
         <v>295</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>296</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="22">
@@ -5059,7 +5059,7 @@
         <v>70</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="R39" s="2" t="s">
         <v>257</v>
@@ -5080,19 +5080,19 @@
         <v>61</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F40" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="H40" s="25" t="s">
         <v>299</v>
-      </c>
-      <c r="H40" s="25" t="s">
-        <v>300</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="22">
@@ -5108,19 +5108,19 @@
         <v>50000</v>
       </c>
       <c r="N40" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P40" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q40" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="R40" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="R40" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="S40" s="2"/>
       <c r="T40" s="41" t="s">
@@ -5138,19 +5138,19 @@
         <v>61</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F41" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="H41" s="25" t="s">
         <v>304</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="H41" s="25" t="s">
-        <v>305</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="22">
@@ -5166,19 +5166,19 @@
         <v>50000</v>
       </c>
       <c r="N41" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P41" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q41" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="R41" s="33" t="s">
         <v>307</v>
-      </c>
-      <c r="R41" s="33" t="s">
-        <v>308</v>
       </c>
       <c r="S41" s="2"/>
       <c r="T41" s="41" t="s">
@@ -5196,19 +5196,19 @@
         <v>61</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F42" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="25" t="s">
         <v>310</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>311</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="22">
@@ -5224,19 +5224,19 @@
         <v>49064</v>
       </c>
       <c r="N42" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P42" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q42" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="R42" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="R42" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="S42" s="2"/>
       <c r="T42" s="41" t="s">
@@ -5254,19 +5254,19 @@
         <v>61</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F43" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" s="25" t="s">
         <v>316</v>
-      </c>
-      <c r="H43" s="25" t="s">
-        <v>317</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="22">
@@ -5282,16 +5282,16 @@
         <v>49850</v>
       </c>
       <c r="N43" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="O43" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>319</v>
       </c>
       <c r="P43" s="2" t="s">
         <v>222</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="R43" s="2" t="s">
         <v>70</v>
@@ -5312,19 +5312,19 @@
         <v>61</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F44" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="25" t="s">
         <v>322</v>
-      </c>
-      <c r="H44" s="25" t="s">
-        <v>323</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="22">
@@ -5340,19 +5340,19 @@
         <v>79997</v>
       </c>
       <c r="N44" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="O44" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="O44" s="2" t="s">
+      <c r="P44" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="P44" s="2" t="s">
+      <c r="Q44" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="Q44" s="29" t="s">
+      <c r="R44" s="33" t="s">
         <v>327</v>
-      </c>
-      <c r="R44" s="33" t="s">
-        <v>328</v>
       </c>
       <c r="S44" s="2"/>
       <c r="T44" s="41" t="s">
@@ -5370,19 +5370,19 @@
         <v>61</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F45" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="25" t="s">
         <v>330</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>331</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="22">
@@ -5398,19 +5398,19 @@
         <v>64864</v>
       </c>
       <c r="N45" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P45" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q45" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="R45" s="36" t="s">
         <v>333</v>
-      </c>
-      <c r="R45" s="36" t="s">
-        <v>334</v>
       </c>
       <c r="S45" s="2"/>
       <c r="T45" s="41" t="s">
@@ -5428,19 +5428,19 @@
         <v>61</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F46" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="25" t="s">
         <v>336</v>
-      </c>
-      <c r="H46" s="25" t="s">
-        <v>337</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="22">
@@ -5456,19 +5456,19 @@
         <v>49074</v>
       </c>
       <c r="N46" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P46" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q46" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="R46" s="33" t="s">
         <v>339</v>
-      </c>
-      <c r="R46" s="33" t="s">
-        <v>340</v>
       </c>
       <c r="S46" s="2"/>
       <c r="T46" s="41" t="s">
@@ -5486,19 +5486,19 @@
         <v>61</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F47" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H47" s="25" t="s">
         <v>342</v>
-      </c>
-      <c r="H47" s="25" t="s">
-        <v>343</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="22">
@@ -5514,19 +5514,19 @@
         <v>37317</v>
       </c>
       <c r="N47" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="O47" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>345</v>
       </c>
       <c r="P47" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="R47" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S47" s="2"/>
       <c r="T47" s="41" t="s">
@@ -5544,19 +5544,19 @@
         <v>61</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F48" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="H48" s="25" t="s">
         <v>348</v>
-      </c>
-      <c r="H48" s="25" t="s">
-        <v>349</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="22">
@@ -5575,16 +5575,16 @@
         <v>228</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P48" s="2" t="s">
         <v>228</v>
       </c>
       <c r="Q48" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="R48" s="33" t="s">
         <v>351</v>
-      </c>
-      <c r="R48" s="33" t="s">
-        <v>352</v>
       </c>
       <c r="S48" s="2"/>
       <c r="T48" s="41" t="s">
@@ -5602,19 +5602,19 @@
         <v>61</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F49" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="H49" s="25" t="s">
         <v>354</v>
-      </c>
-      <c r="H49" s="25" t="s">
-        <v>355</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="22">
@@ -5630,16 +5630,16 @@
         <v>46380</v>
       </c>
       <c r="N49" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="O49" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="P49" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R49" s="33"/>
       <c r="S49" s="2"/>
@@ -5658,19 +5658,19 @@
         <v>61</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F50" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="H50" s="25" t="s">
         <v>360</v>
-      </c>
-      <c r="H50" s="25" t="s">
-        <v>361</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="22">
@@ -5686,19 +5686,19 @@
         <v>62876</v>
       </c>
       <c r="N50" s="27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O50" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="R50" s="33" t="s">
         <v>362</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="Q50" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="R50" s="33" t="s">
-        <v>363</v>
       </c>
       <c r="S50" s="2"/>
       <c r="T50" s="41" t="s">
@@ -5716,19 +5716,19 @@
         <v>61</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F51" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="H51" s="25" t="s">
         <v>365</v>
-      </c>
-      <c r="H51" s="25" t="s">
-        <v>366</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="22">
@@ -5744,19 +5744,19 @@
         <v>35242</v>
       </c>
       <c r="N51" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="O51" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="O51" s="2" t="s">
+      <c r="P51" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="P51" s="2" t="s">
+      <c r="Q51" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="Q51" s="2" t="s">
+      <c r="R51" s="33" t="s">
         <v>370</v>
-      </c>
-      <c r="R51" s="33" t="s">
-        <v>371</v>
       </c>
       <c r="S51" s="2"/>
       <c r="T51" s="41" t="s">
@@ -5774,19 +5774,19 @@
         <v>61</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F52" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="H52" s="25" t="s">
         <v>373</v>
-      </c>
-      <c r="H52" s="25" t="s">
-        <v>374</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="22">
@@ -5802,19 +5802,19 @@
         <v>48686</v>
       </c>
       <c r="N52" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q52" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="R52" s="33" t="s">
         <v>351</v>
-      </c>
-      <c r="R52" s="33" t="s">
-        <v>352</v>
       </c>
       <c r="S52" s="2"/>
       <c r="T52" s="41" t="s">
@@ -5832,19 +5832,19 @@
         <v>61</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F53" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="25" t="s">
         <v>376</v>
-      </c>
-      <c r="H53" s="25" t="s">
-        <v>377</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="22">
@@ -5860,19 +5860,19 @@
         <v>46605</v>
       </c>
       <c r="N53" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="O53" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="O53" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="R53" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="S53" s="2"/>
       <c r="T53" s="41" t="s">
@@ -5890,19 +5890,19 @@
         <v>61</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="F54" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="H54" s="25" t="s">
         <v>382</v>
-      </c>
-      <c r="H54" s="25" t="s">
-        <v>383</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="22">
@@ -5918,19 +5918,19 @@
         <v>61262</v>
       </c>
       <c r="N54" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="P54" s="2" t="s">
         <v>70</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R54" s="33" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S54" s="2"/>
       <c r="T54" s="41" t="s">
@@ -5945,22 +5945,22 @@
         <v>60</v>
       </c>
       <c r="C55" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F55" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="22">
@@ -5979,7 +5979,7 @@
         <v>252</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="P55" s="2" t="s">
         <v>70</v>
@@ -5988,7 +5988,7 @@
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
       <c r="T55" s="41" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="17.25" customHeight="1">
@@ -5999,22 +5999,22 @@
         <v>60</v>
       </c>
       <c r="C56" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F56" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="H56" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="22">
@@ -6033,14 +6033,14 @@
         <v>252</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="41" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="17.25" customHeight="1">
@@ -6051,22 +6051,22 @@
         <v>60</v>
       </c>
       <c r="C57" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F57" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="22">
@@ -6085,14 +6085,14 @@
         <v>252</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
       <c r="T57" s="41" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="17.25" customHeight="1">
@@ -6103,22 +6103,22 @@
         <v>60</v>
       </c>
       <c r="C58" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F58" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="22">
@@ -6137,14 +6137,14 @@
         <v>252</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
       <c r="T58" s="41" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="17.25" customHeight="1">
@@ -6155,22 +6155,22 @@
         <v>60</v>
       </c>
       <c r="C59" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F59" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="22">
@@ -6189,7 +6189,7 @@
         <v>252</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P59" s="2" t="s">
         <v>70</v>
@@ -6198,7 +6198,7 @@
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
       <c r="T59" s="41" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="17.25" customHeight="1">
@@ -6209,22 +6209,22 @@
         <v>60</v>
       </c>
       <c r="C60" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F60" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>415</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="22">
@@ -6243,7 +6243,7 @@
         <v>252</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="P60" s="2" t="s">
         <v>70</v>
@@ -6252,7 +6252,7 @@
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
       <c r="T60" s="41" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="61" spans="1:20" ht="17.25" customHeight="1">
@@ -6263,22 +6263,22 @@
         <v>60</v>
       </c>
       <c r="C61" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F61" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="H61" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>420</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="22">
@@ -6297,14 +6297,14 @@
         <v>252</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
       <c r="T61" s="41" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="62" spans="1:20" ht="17.25" customHeight="1">
@@ -6315,22 +6315,22 @@
         <v>60</v>
       </c>
       <c r="C62" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F62" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="22">
@@ -6349,7 +6349,7 @@
         <v>252</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P62" s="2" t="s">
         <v>70</v>
@@ -6358,7 +6358,7 @@
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
       <c r="T62" s="41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="17.25" customHeight="1">
@@ -6369,22 +6369,22 @@
         <v>60</v>
       </c>
       <c r="C63" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F63" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="22">
@@ -6403,14 +6403,14 @@
         <v>252</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
       <c r="T63" s="41" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="64" spans="1:20" ht="17.25" customHeight="1">
@@ -6421,22 +6421,22 @@
         <v>60</v>
       </c>
       <c r="C64" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F64" s="19" t="s">
+        <v>432</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="H64" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="22">
@@ -6455,14 +6455,14 @@
         <v>252</v>
       </c>
       <c r="O64" s="39" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P64" s="39"/>
       <c r="Q64" s="39"/>
       <c r="R64" s="39"/>
       <c r="S64" s="2"/>
       <c r="T64" s="41" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="65" spans="1:20" ht="17.25" customHeight="1">
@@ -6473,22 +6473,22 @@
         <v>60</v>
       </c>
       <c r="C65" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F65" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="22">
@@ -6507,7 +6507,7 @@
         <v>252</v>
       </c>
       <c r="O65" s="39" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="P65" s="39" t="s">
         <v>70</v>
@@ -6516,7 +6516,7 @@
       <c r="R65" s="39"/>
       <c r="S65" s="2"/>
       <c r="T65" s="41" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="66" spans="1:20" ht="17.25" customHeight="1">
@@ -6527,22 +6527,22 @@
         <v>60</v>
       </c>
       <c r="C66" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F66" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="22">
@@ -6561,14 +6561,14 @@
         <v>252</v>
       </c>
       <c r="O66" s="39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P66" s="39"/>
       <c r="Q66" s="39"/>
       <c r="R66" s="39"/>
       <c r="S66" s="2"/>
       <c r="T66" s="41" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="67" spans="1:20" ht="17.25" customHeight="1">
@@ -6579,22 +6579,22 @@
         <v>60</v>
       </c>
       <c r="C67" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F67" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="H67" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>450</v>
       </c>
       <c r="I67" s="2"/>
       <c r="J67" s="22">
@@ -6613,14 +6613,14 @@
         <v>252</v>
       </c>
       <c r="O67" s="39" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P67" s="39"/>
       <c r="Q67" s="39"/>
       <c r="R67" s="39"/>
       <c r="S67" s="2"/>
       <c r="T67" s="41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="68" spans="1:20" ht="17.25" customHeight="1">
@@ -6631,22 +6631,22 @@
         <v>60</v>
       </c>
       <c r="C68" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F68" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="H68" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>455</v>
       </c>
       <c r="I68" s="2"/>
       <c r="J68" s="22">
@@ -6665,7 +6665,7 @@
         <v>252</v>
       </c>
       <c r="O68" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P68" s="39" t="s">
         <v>70</v>
@@ -6674,7 +6674,7 @@
       <c r="R68" s="39"/>
       <c r="S68" s="2"/>
       <c r="T68" s="41" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="69" spans="1:20" ht="17.25" customHeight="1">
@@ -6685,22 +6685,22 @@
         <v>60</v>
       </c>
       <c r="C69" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F69" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>459</v>
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="22">
@@ -6719,7 +6719,7 @@
         <v>252</v>
       </c>
       <c r="O69" s="39" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P69" s="39" t="s">
         <v>70</v>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="S69" s="2"/>
       <c r="T69" s="41" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="70" spans="1:20" ht="17.25" customHeight="1">
@@ -6741,22 +6741,22 @@
         <v>60</v>
       </c>
       <c r="C70" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F70" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>463</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>464</v>
       </c>
       <c r="I70" s="2"/>
       <c r="J70" s="22">
@@ -6775,14 +6775,14 @@
         <v>252</v>
       </c>
       <c r="O70" s="39" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P70" s="39"/>
       <c r="Q70" s="39"/>
       <c r="R70" s="39"/>
       <c r="S70" s="2"/>
       <c r="T70" s="41" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="71" spans="1:20" ht="17.25" customHeight="1">
@@ -6793,22 +6793,22 @@
         <v>60</v>
       </c>
       <c r="C71" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F71" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="H71" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>469</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="22">
@@ -6827,14 +6827,14 @@
         <v>252</v>
       </c>
       <c r="O71" s="39" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P71" s="39"/>
       <c r="Q71" s="39"/>
       <c r="R71" s="39"/>
       <c r="S71" s="2"/>
       <c r="T71" s="41" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="72" spans="1:20" ht="17.25" customHeight="1">
@@ -6845,22 +6845,22 @@
         <v>60</v>
       </c>
       <c r="C72" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F72" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="H72" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="I72" s="2"/>
       <c r="J72" s="22">
@@ -6879,7 +6879,7 @@
         <v>252</v>
       </c>
       <c r="O72" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P72" s="39" t="s">
         <v>70</v>
@@ -6888,7 +6888,7 @@
       <c r="R72" s="39"/>
       <c r="S72" s="2"/>
       <c r="T72" s="41" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="73" spans="1:20" ht="17.25" customHeight="1">
@@ -6899,22 +6899,22 @@
         <v>60</v>
       </c>
       <c r="C73" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F73" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="H73" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>477</v>
       </c>
       <c r="I73" s="2"/>
       <c r="J73" s="22">
@@ -6933,7 +6933,7 @@
         <v>252</v>
       </c>
       <c r="O73" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P73" s="2" t="s">
         <v>70</v>
@@ -6942,7 +6942,7 @@
       <c r="R73" s="39"/>
       <c r="S73" s="2"/>
       <c r="T73" s="41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="74" spans="1:20" ht="17.25" customHeight="1">
@@ -6953,22 +6953,22 @@
         <v>60</v>
       </c>
       <c r="C74" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F74" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="G74" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" s="22">
@@ -6987,7 +6987,7 @@
         <v>252</v>
       </c>
       <c r="O74" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P74" s="39" t="s">
         <v>70</v>
@@ -6996,7 +6996,7 @@
       <c r="R74" s="39"/>
       <c r="S74" s="2"/>
       <c r="T74" s="41" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="75" spans="1:20" ht="17.25" customHeight="1">
@@ -7007,22 +7007,22 @@
         <v>60</v>
       </c>
       <c r="C75" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F75" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H75" s="39" t="s">
         <v>483</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="H75" s="39" t="s">
-        <v>484</v>
       </c>
       <c r="I75" s="2"/>
       <c r="J75" s="22">
@@ -7041,14 +7041,14 @@
         <v>252</v>
       </c>
       <c r="O75" s="39" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P75" s="39"/>
       <c r="Q75" s="39"/>
       <c r="R75" s="39"/>
       <c r="S75" s="2"/>
       <c r="T75" s="41" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="76" spans="1:20" ht="17.25" customHeight="1">
@@ -7059,22 +7059,22 @@
         <v>60</v>
       </c>
       <c r="C76" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F76" s="42" t="s">
+        <v>485</v>
+      </c>
+      <c r="G76" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>487</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>488</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="22">
@@ -7093,14 +7093,14 @@
         <v>252</v>
       </c>
       <c r="O76" s="39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P76" s="39"/>
       <c r="Q76" s="39"/>
       <c r="R76" s="39"/>
       <c r="S76" s="2"/>
       <c r="T76" s="41" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="77" spans="1:20" ht="17.25" customHeight="1">
@@ -7111,22 +7111,22 @@
         <v>60</v>
       </c>
       <c r="C77" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D77" s="39" t="s">
         <v>386</v>
-      </c>
-      <c r="D77" s="39" t="s">
-        <v>387</v>
       </c>
       <c r="E77" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F77" s="42" t="s">
+        <v>489</v>
+      </c>
+      <c r="G77" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="H77" s="39" t="s">
         <v>491</v>
-      </c>
-      <c r="H77" s="39" t="s">
-        <v>492</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="22">
@@ -7145,14 +7145,14 @@
         <v>252</v>
       </c>
       <c r="O77" s="39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P77" s="39"/>
       <c r="Q77" s="39"/>
       <c r="R77" s="39"/>
       <c r="S77" s="2"/>
       <c r="T77" s="41" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="78" spans="1:20" ht="17.25" customHeight="1">
@@ -7163,22 +7163,22 @@
         <v>60</v>
       </c>
       <c r="C78" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D78" s="39" t="s">
         <v>386</v>
-      </c>
-      <c r="D78" s="39" t="s">
-        <v>387</v>
       </c>
       <c r="E78" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F78" s="42" t="s">
+        <v>493</v>
+      </c>
+      <c r="G78" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="H78" s="39" t="s">
         <v>495</v>
-      </c>
-      <c r="H78" s="39" t="s">
-        <v>496</v>
       </c>
       <c r="I78" s="2"/>
       <c r="J78" s="22">
@@ -7197,14 +7197,14 @@
         <v>252</v>
       </c>
       <c r="O78" s="39" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P78" s="39"/>
       <c r="Q78" s="39"/>
       <c r="R78" s="39"/>
       <c r="S78" s="2"/>
       <c r="T78" s="41" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="79" spans="1:20" ht="17.25" customHeight="1">
@@ -7215,19 +7215,19 @@
         <v>60</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D79" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="E79" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="39" t="s">
+      <c r="F79" s="42" t="s">
         <v>499</v>
       </c>
-      <c r="F79" s="42" t="s">
+      <c r="G79" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="H79" s="39"/>
       <c r="I79" s="2"/>
@@ -7245,14 +7245,14 @@
         <v>252</v>
       </c>
       <c r="O79" s="39" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="P79" s="39"/>
       <c r="Q79" s="39"/>
       <c r="R79" s="39"/>
       <c r="S79" s="2"/>
       <c r="T79" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="80" spans="1:20" ht="17.25" customHeight="1">
@@ -7263,19 +7263,19 @@
         <v>60</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D80" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="E80" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="E80" s="39" t="s">
-        <v>499</v>
-      </c>
       <c r="F80" s="42" t="s">
+        <v>503</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>505</v>
       </c>
       <c r="H80" s="39"/>
       <c r="I80" s="2"/>
@@ -7293,14 +7293,14 @@
         <v>252</v>
       </c>
       <c r="O80" s="39" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P80" s="39"/>
       <c r="Q80" s="39"/>
       <c r="R80" s="39"/>
       <c r="S80" s="2"/>
       <c r="T80" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="81" spans="1:20" ht="17.25" customHeight="1">
@@ -7311,19 +7311,19 @@
         <v>60</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D81" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="E81" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="E81" s="39" t="s">
-        <v>499</v>
-      </c>
       <c r="F81" s="42" t="s">
+        <v>506</v>
+      </c>
+      <c r="G81" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>508</v>
       </c>
       <c r="H81" s="39"/>
       <c r="I81" s="2"/>
@@ -7341,14 +7341,14 @@
         <v>252</v>
       </c>
       <c r="O81" s="39" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="P81" s="39"/>
       <c r="Q81" s="39"/>
       <c r="R81" s="39"/>
       <c r="S81" s="2"/>
       <c r="T81" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="82" spans="1:20" ht="17.25" customHeight="1">
@@ -7359,19 +7359,19 @@
         <v>60</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D82" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="E82" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="E82" s="39" t="s">
-        <v>499</v>
-      </c>
       <c r="F82" s="42" t="s">
+        <v>509</v>
+      </c>
+      <c r="G82" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>511</v>
       </c>
       <c r="H82" s="39"/>
       <c r="I82" s="2"/>
@@ -7389,14 +7389,14 @@
         <v>252</v>
       </c>
       <c r="O82" s="39" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P82" s="39"/>
       <c r="Q82" s="39"/>
       <c r="R82" s="39"/>
       <c r="S82" s="2"/>
       <c r="T82" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="83" spans="1:20" ht="17.25" customHeight="1">
@@ -7407,19 +7407,19 @@
         <v>60</v>
       </c>
       <c r="C83" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D83" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="E83" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="E83" s="39" t="s">
-        <v>499</v>
-      </c>
       <c r="F83" s="42" t="s">
+        <v>512</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>513</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>514</v>
       </c>
       <c r="H83" s="39"/>
       <c r="I83" s="2"/>
@@ -7437,14 +7437,14 @@
         <v>252</v>
       </c>
       <c r="O83" s="39" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P83" s="39"/>
       <c r="Q83" s="39"/>
       <c r="R83" s="39"/>
       <c r="S83" s="2"/>
       <c r="T83" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="84" spans="1:20" ht="17.25" customHeight="1">
@@ -7455,19 +7455,19 @@
         <v>60</v>
       </c>
       <c r="C84" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D84" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="E84" s="39" t="s">
         <v>498</v>
       </c>
-      <c r="E84" s="39" t="s">
-        <v>499</v>
-      </c>
       <c r="F84" s="42" t="s">
+        <v>515</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>517</v>
       </c>
       <c r="H84" s="39"/>
       <c r="I84" s="2"/>
@@ -7483,14 +7483,14 @@
         <v>252</v>
       </c>
       <c r="O84" s="39" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P84" s="39"/>
       <c r="Q84" s="39"/>
       <c r="R84" s="39"/>
       <c r="S84" s="2"/>
       <c r="T84" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="85" spans="1:20" ht="17.25" customHeight="1">
@@ -7501,22 +7501,22 @@
         <v>60</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D85" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E85" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F85" s="42" t="s">
+        <v>519</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="H85" s="39" t="s">
         <v>521</v>
-      </c>
-      <c r="H85" s="39" t="s">
-        <v>522</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="22">
@@ -7535,7 +7535,7 @@
         <v>252</v>
       </c>
       <c r="O85" s="39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P85" s="39" t="s">
         <v>70</v>
@@ -7548,7 +7548,7 @@
       </c>
       <c r="S85" s="2"/>
       <c r="T85" s="41" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="86" spans="1:20" ht="17.25" customHeight="1">
@@ -7559,22 +7559,22 @@
         <v>60</v>
       </c>
       <c r="C86" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D86" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E86" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F86" s="42" t="s">
+        <v>523</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="H86" s="39" t="s">
         <v>525</v>
-      </c>
-      <c r="H86" s="39" t="s">
-        <v>526</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="22">
@@ -7593,7 +7593,7 @@
         <v>252</v>
       </c>
       <c r="O86" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P86" s="2" t="s">
         <v>70</v>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="S86" s="2"/>
       <c r="T86" s="41" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="87" spans="1:20" ht="17.25" customHeight="1">
@@ -7617,22 +7617,22 @@
         <v>60</v>
       </c>
       <c r="C87" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D87" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E87" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F87" s="42" t="s">
+        <v>527</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="H87" s="39" t="s">
         <v>529</v>
-      </c>
-      <c r="H87" s="39" t="s">
-        <v>530</v>
       </c>
       <c r="I87" s="2"/>
       <c r="J87" s="22">
@@ -7651,14 +7651,14 @@
         <v>252</v>
       </c>
       <c r="O87" s="39" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P87" s="39"/>
       <c r="Q87" s="39"/>
       <c r="R87" s="39"/>
       <c r="S87" s="2"/>
       <c r="T87" s="41" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="88" spans="1:20" ht="17.25" customHeight="1">
@@ -7669,22 +7669,22 @@
         <v>60</v>
       </c>
       <c r="C88" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D88" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E88" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F88" s="42" t="s">
+        <v>531</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="G88" s="2" t="s">
+      <c r="H88" s="39" t="s">
         <v>533</v>
-      </c>
-      <c r="H88" s="39" t="s">
-        <v>534</v>
       </c>
       <c r="I88" s="2"/>
       <c r="J88" s="22">
@@ -7703,7 +7703,7 @@
         <v>252</v>
       </c>
       <c r="O88" s="39" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="P88" s="2" t="s">
         <v>70</v>
@@ -7712,7 +7712,7 @@
       <c r="R88" s="39"/>
       <c r="S88" s="2"/>
       <c r="T88" s="41" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="89" spans="1:20" ht="17.25" customHeight="1">
@@ -7723,22 +7723,22 @@
         <v>60</v>
       </c>
       <c r="C89" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D89" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E89" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F89" s="42" t="s">
+        <v>535</v>
+      </c>
+      <c r="G89" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="G89" s="2" t="s">
+      <c r="H89" s="39" t="s">
         <v>537</v>
-      </c>
-      <c r="H89" s="39" t="s">
-        <v>538</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="22">
@@ -7757,7 +7757,7 @@
         <v>252</v>
       </c>
       <c r="O89" s="39" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="P89" s="39" t="s">
         <v>70</v>
@@ -7766,7 +7766,7 @@
       <c r="R89" s="39"/>
       <c r="S89" s="2"/>
       <c r="T89" s="41" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="90" spans="1:20" ht="17.25" customHeight="1">
@@ -7777,22 +7777,22 @@
         <v>60</v>
       </c>
       <c r="C90" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D90" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E90" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F90" s="42" t="s">
+        <v>539</v>
+      </c>
+      <c r="G90" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="H90" s="39" t="s">
         <v>541</v>
-      </c>
-      <c r="H90" s="39" t="s">
-        <v>542</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="22">
@@ -7811,14 +7811,14 @@
         <v>252</v>
       </c>
       <c r="O90" s="39" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="P90" s="39"/>
       <c r="Q90" s="39"/>
       <c r="R90" s="39"/>
       <c r="S90" s="2"/>
       <c r="T90" s="41" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="91" spans="1:20" ht="17.25" customHeight="1">
@@ -7829,22 +7829,22 @@
         <v>60</v>
       </c>
       <c r="C91" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D91" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E91" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F91" s="42" t="s">
+        <v>544</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="H91" s="39" t="s">
         <v>546</v>
-      </c>
-      <c r="H91" s="39" t="s">
-        <v>547</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="22">
@@ -7863,14 +7863,14 @@
         <v>252</v>
       </c>
       <c r="O91" s="39" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="P91" s="39"/>
       <c r="Q91" s="39"/>
       <c r="R91" s="39"/>
       <c r="S91" s="2"/>
       <c r="T91" s="41" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="92" spans="1:20" ht="17.25" customHeight="1">
@@ -7881,22 +7881,22 @@
         <v>60</v>
       </c>
       <c r="C92" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D92" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E92" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F92" s="42" t="s">
+        <v>549</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="H92" s="39" t="s">
         <v>551</v>
-      </c>
-      <c r="H92" s="39" t="s">
-        <v>552</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="22">
@@ -7915,7 +7915,7 @@
         <v>252</v>
       </c>
       <c r="O92" s="39" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P92" s="2" t="s">
         <v>70</v>
@@ -7924,7 +7924,7 @@
       <c r="R92" s="39"/>
       <c r="S92" s="2"/>
       <c r="T92" s="41" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="93" spans="1:20" ht="17.25" customHeight="1">
@@ -7935,22 +7935,22 @@
         <v>60</v>
       </c>
       <c r="C93" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D93" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E93" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F93" s="42" t="s">
+        <v>553</v>
+      </c>
+      <c r="G93" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="G93" s="2" t="s">
+      <c r="H93" s="39" t="s">
         <v>555</v>
-      </c>
-      <c r="H93" s="39" t="s">
-        <v>556</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="22">
@@ -7969,7 +7969,7 @@
         <v>252</v>
       </c>
       <c r="O93" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P93" s="39" t="s">
         <v>70</v>
@@ -7978,7 +7978,7 @@
       <c r="R93" s="39"/>
       <c r="S93" s="2"/>
       <c r="T93" s="41" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="94" spans="1:20" ht="17.25" customHeight="1">
@@ -7989,22 +7989,22 @@
         <v>60</v>
       </c>
       <c r="C94" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D94" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E94" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F94" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="G94" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="H94" s="39" t="s">
         <v>559</v>
-      </c>
-      <c r="H94" s="39" t="s">
-        <v>560</v>
       </c>
       <c r="I94" s="2"/>
       <c r="J94" s="22">
@@ -8023,7 +8023,7 @@
         <v>252</v>
       </c>
       <c r="O94" s="39" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="P94" s="39" t="s">
         <v>70</v>
@@ -8036,7 +8036,7 @@
       </c>
       <c r="S94" s="2"/>
       <c r="T94" s="41" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="95" spans="1:20" ht="17.25" customHeight="1">
@@ -8047,22 +8047,22 @@
         <v>60</v>
       </c>
       <c r="C95" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D95" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E95" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F95" s="42" t="s">
+        <v>562</v>
+      </c>
+      <c r="G95" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="H95" s="39" t="s">
         <v>564</v>
-      </c>
-      <c r="H95" s="39" t="s">
-        <v>565</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="22">
@@ -8081,7 +8081,7 @@
         <v>252</v>
       </c>
       <c r="O95" s="39" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="P95" s="39"/>
       <c r="Q95" s="39"/>
@@ -8090,7 +8090,7 @@
       </c>
       <c r="S95" s="2"/>
       <c r="T95" s="41" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="96" spans="1:20" ht="17.25" customHeight="1">
@@ -8101,22 +8101,22 @@
         <v>60</v>
       </c>
       <c r="C96" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D96" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E96" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F96" s="42" t="s">
+        <v>567</v>
+      </c>
+      <c r="G96" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="H96" s="39" t="s">
         <v>569</v>
-      </c>
-      <c r="H96" s="39" t="s">
-        <v>570</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="22">
@@ -8135,7 +8135,7 @@
         <v>252</v>
       </c>
       <c r="O96" s="39" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="P96" s="39"/>
       <c r="Q96" s="39"/>
@@ -8144,7 +8144,7 @@
       </c>
       <c r="S96" s="2"/>
       <c r="T96" s="41" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="97" spans="1:20" ht="17.25" customHeight="1">
@@ -8155,22 +8155,22 @@
         <v>60</v>
       </c>
       <c r="C97" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D97" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E97" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F97" s="42" t="s">
+        <v>572</v>
+      </c>
+      <c r="G97" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="G97" s="2" t="s">
+      <c r="H97" s="39" t="s">
         <v>574</v>
-      </c>
-      <c r="H97" s="39" t="s">
-        <v>575</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="22">
@@ -8189,7 +8189,7 @@
         <v>252</v>
       </c>
       <c r="O97" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P97" s="39" t="s">
         <v>70</v>
@@ -8202,7 +8202,7 @@
       </c>
       <c r="S97" s="2"/>
       <c r="T97" s="41" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="98" spans="1:20" ht="17.25" customHeight="1">
@@ -8213,22 +8213,22 @@
         <v>60</v>
       </c>
       <c r="C98" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D98" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E98" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F98" s="42" t="s">
+        <v>576</v>
+      </c>
+      <c r="G98" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="G98" s="2" t="s">
-        <v>578</v>
-      </c>
       <c r="H98" s="39" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I98" s="2"/>
       <c r="J98" s="22">
@@ -8247,7 +8247,7 @@
         <v>252</v>
       </c>
       <c r="O98" s="39" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="P98" s="39" t="s">
         <v>70</v>
@@ -8256,7 +8256,7 @@
       <c r="R98" s="39"/>
       <c r="S98" s="2"/>
       <c r="T98" s="41" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="99" spans="1:20" ht="17.25" customHeight="1">
@@ -8267,22 +8267,22 @@
         <v>60</v>
       </c>
       <c r="C99" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D99" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E99" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F99" s="42" t="s">
+        <v>579</v>
+      </c>
+      <c r="G99" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="G99" s="2" t="s">
-        <v>581</v>
-      </c>
       <c r="H99" s="39" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I99" s="2"/>
       <c r="J99" s="22">
@@ -8301,7 +8301,7 @@
         <v>252</v>
       </c>
       <c r="O99" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P99" s="2" t="s">
         <v>70</v>
@@ -8310,7 +8310,7 @@
       <c r="R99" s="39"/>
       <c r="S99" s="2"/>
       <c r="T99" s="41" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="100" spans="1:20" ht="17.25" customHeight="1">
@@ -8321,22 +8321,22 @@
         <v>60</v>
       </c>
       <c r="C100" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D100" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E100" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F100" s="42" t="s">
+        <v>582</v>
+      </c>
+      <c r="G100" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="H100" s="39" t="s">
         <v>584</v>
-      </c>
-      <c r="H100" s="39" t="s">
-        <v>585</v>
       </c>
       <c r="I100" s="2"/>
       <c r="J100" s="22">
@@ -8355,7 +8355,7 @@
         <v>252</v>
       </c>
       <c r="O100" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P100" s="39" t="s">
         <v>70</v>
@@ -8368,7 +8368,7 @@
       </c>
       <c r="S100" s="2"/>
       <c r="T100" s="41" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="101" spans="1:20" ht="17.25" customHeight="1">
@@ -8379,22 +8379,22 @@
         <v>60</v>
       </c>
       <c r="C101" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D101" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E101" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F101" s="42" t="s">
+        <v>586</v>
+      </c>
+      <c r="G101" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="H101" s="39" t="s">
         <v>588</v>
-      </c>
-      <c r="H101" s="39" t="s">
-        <v>589</v>
       </c>
       <c r="I101" s="2"/>
       <c r="J101" s="22">
@@ -8413,14 +8413,14 @@
         <v>252</v>
       </c>
       <c r="O101" s="39" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P101" s="39"/>
       <c r="Q101" s="39"/>
       <c r="R101" s="39"/>
       <c r="S101" s="2"/>
       <c r="T101" s="41" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="102" spans="1:20" ht="17.25" customHeight="1">
@@ -8431,22 +8431,22 @@
         <v>60</v>
       </c>
       <c r="C102" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D102" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E102" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F102" s="42" t="s">
+        <v>591</v>
+      </c>
+      <c r="G102" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="H102" s="39" t="s">
         <v>593</v>
-      </c>
-      <c r="H102" s="39" t="s">
-        <v>594</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="22">
@@ -8465,14 +8465,14 @@
         <v>252</v>
       </c>
       <c r="O102" s="39" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P102" s="39"/>
       <c r="Q102" s="39"/>
       <c r="R102" s="39"/>
       <c r="S102" s="2"/>
       <c r="T102" s="41" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="103" spans="1:20" ht="17.25" customHeight="1">
@@ -8483,22 +8483,22 @@
         <v>60</v>
       </c>
       <c r="C103" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D103" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E103" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F103" s="42" t="s">
+        <v>596</v>
+      </c>
+      <c r="G103" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="G103" s="2" t="s">
-        <v>598</v>
-      </c>
       <c r="H103" s="39" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="22">
@@ -8517,7 +8517,7 @@
         <v>252</v>
       </c>
       <c r="O103" s="39" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P103" s="39" t="s">
         <v>70</v>
@@ -8526,7 +8526,7 @@
       <c r="R103" s="39"/>
       <c r="S103" s="2"/>
       <c r="T103" s="41" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="104" spans="1:20" ht="17.25" customHeight="1">
@@ -8537,22 +8537,22 @@
         <v>60</v>
       </c>
       <c r="C104" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D104" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E104" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F104" s="42" t="s">
+        <v>600</v>
+      </c>
+      <c r="G104" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="G104" s="2" t="s">
-        <v>602</v>
-      </c>
       <c r="H104" s="39" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="22">
@@ -8571,14 +8571,14 @@
         <v>252</v>
       </c>
       <c r="O104" s="39" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P104" s="39"/>
       <c r="Q104" s="39"/>
       <c r="R104" s="39"/>
       <c r="S104" s="2"/>
       <c r="T104" s="41" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="105" spans="1:20" ht="17.25" customHeight="1">
@@ -8589,22 +8589,22 @@
         <v>60</v>
       </c>
       <c r="C105" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D105" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E105" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F105" s="42" t="s">
+        <v>604</v>
+      </c>
+      <c r="G105" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="G105" s="2" t="s">
-        <v>606</v>
-      </c>
       <c r="H105" s="39" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="22">
@@ -8623,7 +8623,7 @@
         <v>252</v>
       </c>
       <c r="O105" s="39" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="P105" s="39" t="s">
         <v>70</v>
@@ -8632,7 +8632,7 @@
       <c r="R105" s="39"/>
       <c r="S105" s="2"/>
       <c r="T105" s="41" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="106" spans="1:20" ht="17.25" customHeight="1">
@@ -8643,22 +8643,22 @@
         <v>60</v>
       </c>
       <c r="C106" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D106" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E106" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F106" s="42" t="s">
+        <v>608</v>
+      </c>
+      <c r="G106" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="G106" s="2" t="s">
+      <c r="H106" s="39" t="s">
         <v>610</v>
-      </c>
-      <c r="H106" s="39" t="s">
-        <v>611</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="22">
@@ -8677,7 +8677,7 @@
         <v>252</v>
       </c>
       <c r="O106" s="39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P106" s="39" t="s">
         <v>70</v>
@@ -8686,7 +8686,7 @@
       <c r="R106" s="39"/>
       <c r="S106" s="2"/>
       <c r="T106" s="41" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="107" spans="1:20" ht="17.25" customHeight="1">
@@ -8697,22 +8697,22 @@
         <v>60</v>
       </c>
       <c r="C107" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D107" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E107" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F107" s="42" t="s">
+        <v>612</v>
+      </c>
+      <c r="G107" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="G107" s="2" t="s">
+      <c r="H107" s="39" t="s">
         <v>614</v>
-      </c>
-      <c r="H107" s="39" t="s">
-        <v>615</v>
       </c>
       <c r="I107" s="2"/>
       <c r="J107" s="22">
@@ -8731,14 +8731,14 @@
         <v>252</v>
       </c>
       <c r="O107" s="39" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="P107" s="39"/>
       <c r="Q107" s="39"/>
       <c r="R107" s="39"/>
       <c r="S107" s="2"/>
       <c r="T107" s="41" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="108" spans="1:20" ht="17.25" customHeight="1">
@@ -8749,22 +8749,22 @@
         <v>60</v>
       </c>
       <c r="C108" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D108" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E108" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F108" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="G108" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="H108" s="39" t="s">
         <v>619</v>
-      </c>
-      <c r="H108" s="39" t="s">
-        <v>620</v>
       </c>
       <c r="I108" s="2"/>
       <c r="J108" s="22">
@@ -8783,7 +8783,7 @@
         <v>252</v>
       </c>
       <c r="O108" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P108" s="39" t="s">
         <v>70</v>
@@ -8792,7 +8792,7 @@
       <c r="R108" s="39"/>
       <c r="S108" s="2"/>
       <c r="T108" s="41" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="109" spans="1:20" ht="17.25" customHeight="1">
@@ -8803,22 +8803,22 @@
         <v>60</v>
       </c>
       <c r="C109" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D109" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E109" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F109" s="42" t="s">
+        <v>621</v>
+      </c>
+      <c r="G109" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="G109" s="2" t="s">
+      <c r="H109" s="39" t="s">
         <v>623</v>
-      </c>
-      <c r="H109" s="39" t="s">
-        <v>624</v>
       </c>
       <c r="I109" s="2"/>
       <c r="J109" s="22">
@@ -8837,7 +8837,7 @@
         <v>252</v>
       </c>
       <c r="O109" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P109" s="39" t="s">
         <v>70</v>
@@ -8846,7 +8846,7 @@
       <c r="R109" s="39"/>
       <c r="S109" s="2"/>
       <c r="T109" s="41" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="110" spans="1:20" ht="17.25" customHeight="1">
@@ -8857,22 +8857,22 @@
         <v>60</v>
       </c>
       <c r="C110" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D110" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E110" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F110" s="42" t="s">
+        <v>625</v>
+      </c>
+      <c r="G110" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="H110" s="39" t="s">
         <v>627</v>
-      </c>
-      <c r="H110" s="39" t="s">
-        <v>628</v>
       </c>
       <c r="I110" s="2"/>
       <c r="J110" s="22">
@@ -8891,7 +8891,7 @@
         <v>252</v>
       </c>
       <c r="O110" s="39" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="P110" s="39" t="s">
         <v>70</v>
@@ -8900,7 +8900,7 @@
       <c r="R110" s="39"/>
       <c r="S110" s="2"/>
       <c r="T110" s="41" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="111" spans="1:20" ht="17.25" customHeight="1">
@@ -8911,22 +8911,22 @@
         <v>60</v>
       </c>
       <c r="C111" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D111" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E111" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F111" s="42" t="s">
+        <v>629</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="H111" s="39" t="s">
         <v>630</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="H111" s="39" t="s">
-        <v>631</v>
       </c>
       <c r="I111" s="2"/>
       <c r="J111" s="22">
@@ -8945,7 +8945,7 @@
         <v>252</v>
       </c>
       <c r="O111" s="39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P111" s="39" t="s">
         <v>70</v>
@@ -8954,7 +8954,7 @@
       <c r="R111" s="39"/>
       <c r="S111" s="2"/>
       <c r="T111" s="41" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="112" spans="1:20" ht="17.25" customHeight="1">
@@ -8965,22 +8965,22 @@
         <v>60</v>
       </c>
       <c r="C112" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D112" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E112" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F112" s="42" t="s">
+        <v>632</v>
+      </c>
+      <c r="G112" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="G112" s="2" t="s">
+      <c r="H112" s="39" t="s">
         <v>634</v>
-      </c>
-      <c r="H112" s="39" t="s">
-        <v>635</v>
       </c>
       <c r="I112" s="2"/>
       <c r="J112" s="22">
@@ -8999,7 +8999,7 @@
         <v>252</v>
       </c>
       <c r="O112" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P112" s="2" t="s">
         <v>70</v>
@@ -9008,7 +9008,7 @@
       <c r="R112" s="39"/>
       <c r="S112" s="2"/>
       <c r="T112" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="113" spans="1:20" ht="17.25" customHeight="1">
@@ -9019,22 +9019,22 @@
         <v>60</v>
       </c>
       <c r="C113" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D113" s="39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E113" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F113" s="42" t="s">
+        <v>636</v>
+      </c>
+      <c r="G113" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="G113" s="2" t="s">
+      <c r="H113" s="39" t="s">
         <v>638</v>
-      </c>
-      <c r="H113" s="39" t="s">
-        <v>639</v>
       </c>
       <c r="I113" s="2"/>
       <c r="J113" s="22">
@@ -9053,7 +9053,7 @@
         <v>252</v>
       </c>
       <c r="O113" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P113" s="39" t="s">
         <v>70</v>
@@ -9062,7 +9062,7 @@
       <c r="R113" s="39"/>
       <c r="S113" s="2"/>
       <c r="T113" s="41" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="114" spans="1:20" ht="17.25" customHeight="1">
@@ -9073,22 +9073,22 @@
         <v>60</v>
       </c>
       <c r="C114" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D114" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E114" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F114" s="42" t="s">
+        <v>641</v>
+      </c>
+      <c r="G114" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="H114" s="39" t="s">
         <v>643</v>
-      </c>
-      <c r="H114" s="39" t="s">
-        <v>644</v>
       </c>
       <c r="I114" s="2"/>
       <c r="J114" s="22">
@@ -9107,14 +9107,14 @@
         <v>252</v>
       </c>
       <c r="O114" s="39" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P114" s="39"/>
       <c r="Q114" s="39"/>
       <c r="R114" s="39"/>
       <c r="S114" s="2"/>
       <c r="T114" s="41" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="115" spans="1:20" ht="17.25" customHeight="1">
@@ -9125,22 +9125,22 @@
         <v>60</v>
       </c>
       <c r="C115" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D115" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E115" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F115" s="42" t="s">
+        <v>645</v>
+      </c>
+      <c r="G115" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="G115" s="2" t="s">
+      <c r="H115" s="39" t="s">
         <v>647</v>
-      </c>
-      <c r="H115" s="39" t="s">
-        <v>648</v>
       </c>
       <c r="I115" s="2"/>
       <c r="J115" s="22">
@@ -9159,7 +9159,7 @@
         <v>252</v>
       </c>
       <c r="O115" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P115" s="39" t="s">
         <v>70</v>
@@ -9168,7 +9168,7 @@
       <c r="R115" s="39"/>
       <c r="S115" s="2"/>
       <c r="T115" s="41" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="116" spans="1:20" ht="17.25" customHeight="1">
@@ -9179,22 +9179,22 @@
         <v>60</v>
       </c>
       <c r="C116" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D116" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E116" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F116" s="42" t="s">
+        <v>649</v>
+      </c>
+      <c r="G116" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="G116" s="2" t="s">
+      <c r="H116" s="39" t="s">
         <v>651</v>
-      </c>
-      <c r="H116" s="39" t="s">
-        <v>652</v>
       </c>
       <c r="I116" s="2"/>
       <c r="J116" s="22">
@@ -9213,7 +9213,7 @@
         <v>252</v>
       </c>
       <c r="O116" s="39" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P116" s="39" t="s">
         <v>70</v>
@@ -9222,7 +9222,7 @@
       <c r="R116" s="39"/>
       <c r="S116" s="2"/>
       <c r="T116" s="41" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="117" spans="1:20" ht="17.25" customHeight="1">
@@ -9233,22 +9233,22 @@
         <v>60</v>
       </c>
       <c r="C117" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D117" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E117" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F117" s="42" t="s">
+        <v>653</v>
+      </c>
+      <c r="G117" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="H117" s="39" t="s">
         <v>655</v>
-      </c>
-      <c r="H117" s="39" t="s">
-        <v>656</v>
       </c>
       <c r="I117" s="2"/>
       <c r="J117" s="22">
@@ -9267,7 +9267,7 @@
         <v>252</v>
       </c>
       <c r="O117" s="39" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="P117" s="39" t="s">
         <v>70</v>
@@ -9276,7 +9276,7 @@
       <c r="R117" s="39"/>
       <c r="S117" s="2"/>
       <c r="T117" s="41" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="118" spans="1:20" ht="17.25" customHeight="1">
@@ -9287,22 +9287,22 @@
         <v>60</v>
       </c>
       <c r="C118" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D118" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E118" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F118" s="42" t="s">
+        <v>658</v>
+      </c>
+      <c r="G118" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="H118" s="39" t="s">
         <v>660</v>
-      </c>
-      <c r="H118" s="39" t="s">
-        <v>661</v>
       </c>
       <c r="I118" s="2"/>
       <c r="J118" s="22">
@@ -9321,14 +9321,14 @@
         <v>252</v>
       </c>
       <c r="O118" s="39" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="P118" s="39"/>
       <c r="Q118" s="39"/>
       <c r="R118" s="39"/>
       <c r="S118" s="2"/>
       <c r="T118" s="41" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="119" spans="1:20" ht="17.25" customHeight="1">
@@ -9339,22 +9339,22 @@
         <v>60</v>
       </c>
       <c r="C119" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D119" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E119" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F119" s="42" t="s">
+        <v>663</v>
+      </c>
+      <c r="G119" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="H119" s="39" t="s">
         <v>665</v>
-      </c>
-      <c r="H119" s="39" t="s">
-        <v>666</v>
       </c>
       <c r="I119" s="2"/>
       <c r="J119" s="22">
@@ -9373,7 +9373,7 @@
         <v>252</v>
       </c>
       <c r="O119" s="39" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="P119" s="39" t="s">
         <v>70</v>
@@ -9382,7 +9382,7 @@
       <c r="R119" s="39"/>
       <c r="S119" s="2"/>
       <c r="T119" s="41" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="120" spans="1:20" ht="17.25" customHeight="1">
@@ -9393,22 +9393,22 @@
         <v>60</v>
       </c>
       <c r="C120" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D120" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E120" s="39" t="s">
         <v>63</v>
       </c>
       <c r="F120" s="42" t="s">
+        <v>667</v>
+      </c>
+      <c r="G120" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="G120" s="2" t="s">
+      <c r="H120" s="39" t="s">
         <v>669</v>
-      </c>
-      <c r="H120" s="39" t="s">
-        <v>670</v>
       </c>
       <c r="I120" s="2"/>
       <c r="J120" s="22">
@@ -9427,7 +9427,7 @@
         <v>252</v>
       </c>
       <c r="O120" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P120" s="39" t="s">
         <v>70</v>
@@ -9436,7 +9436,7 @@
       <c r="R120" s="39"/>
       <c r="S120" s="2"/>
       <c r="T120" s="41" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="121" spans="1:20" ht="17.25" customHeight="1">
@@ -9447,19 +9447,19 @@
         <v>60</v>
       </c>
       <c r="C121" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D121" s="39" t="s">
+        <v>671</v>
+      </c>
+      <c r="E121" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="F121" s="42" t="s">
         <v>672</v>
       </c>
-      <c r="E121" s="39" t="s">
-        <v>499</v>
-      </c>
-      <c r="F121" s="42" t="s">
+      <c r="G121" s="2" t="s">
         <v>673</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>674</v>
       </c>
       <c r="H121" s="39"/>
       <c r="I121" s="2"/>
@@ -9477,7 +9477,7 @@
         <v>252</v>
       </c>
       <c r="O121" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P121" s="39" t="s">
         <v>70</v>
@@ -9486,7 +9486,7 @@
       <c r="R121" s="39"/>
       <c r="S121" s="2"/>
       <c r="T121" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="122" spans="1:20" ht="17.25" customHeight="1">
@@ -9497,19 +9497,19 @@
         <v>60</v>
       </c>
       <c r="C122" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D122" s="39" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E122" s="39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F122" s="42" t="s">
+        <v>674</v>
+      </c>
+      <c r="G122" s="2" t="s">
         <v>675</v>
-      </c>
-      <c r="G122" s="2" t="s">
-        <v>676</v>
       </c>
       <c r="H122" s="39"/>
       <c r="I122" s="2"/>
@@ -9527,7 +9527,7 @@
         <v>252</v>
       </c>
       <c r="O122" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P122" s="39" t="s">
         <v>70</v>
@@ -9536,7 +9536,7 @@
       <c r="R122" s="39"/>
       <c r="S122" s="2"/>
       <c r="T122" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="123" spans="1:20" ht="17.25" customHeight="1">
@@ -9547,19 +9547,19 @@
         <v>60</v>
       </c>
       <c r="C123" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D123" s="39" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E123" s="39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F123" s="42" t="s">
+        <v>676</v>
+      </c>
+      <c r="G123" s="2" t="s">
         <v>677</v>
-      </c>
-      <c r="G123" s="2" t="s">
-        <v>678</v>
       </c>
       <c r="H123" s="39"/>
       <c r="I123" s="2"/>
@@ -9577,7 +9577,7 @@
         <v>252</v>
       </c>
       <c r="O123" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P123" s="39" t="s">
         <v>70</v>
@@ -9586,7 +9586,7 @@
       <c r="R123" s="39"/>
       <c r="S123" s="2"/>
       <c r="T123" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="124" spans="1:20" ht="17.25" customHeight="1">
@@ -9597,19 +9597,19 @@
         <v>60</v>
       </c>
       <c r="C124" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D124" s="39" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E124" s="39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F124" s="42" t="s">
+        <v>678</v>
+      </c>
+      <c r="G124" s="2" t="s">
         <v>679</v>
-      </c>
-      <c r="G124" s="2" t="s">
-        <v>680</v>
       </c>
       <c r="H124" s="39"/>
       <c r="I124" s="2"/>
@@ -9627,7 +9627,7 @@
         <v>252</v>
       </c>
       <c r="O124" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P124" s="39" t="s">
         <v>70</v>
@@ -9636,7 +9636,7 @@
       <c r="R124" s="39"/>
       <c r="S124" s="2"/>
       <c r="T124" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="125" spans="1:20" ht="17.25" customHeight="1">
@@ -9647,19 +9647,19 @@
         <v>60</v>
       </c>
       <c r="C125" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D125" s="39" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E125" s="39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F125" s="42" t="s">
+        <v>680</v>
+      </c>
+      <c r="G125" s="2" t="s">
         <v>681</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="H125" s="39"/>
       <c r="I125" s="2"/>
@@ -9677,7 +9677,7 @@
         <v>252</v>
       </c>
       <c r="O125" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P125" s="39" t="s">
         <v>70</v>
@@ -9686,7 +9686,7 @@
       <c r="R125" s="39"/>
       <c r="S125" s="2"/>
       <c r="T125" s="41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="126" spans="1:20" ht="13.5" customHeight="1">
@@ -27893,7 +27893,6 @@
       <c r="T988" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T125" xr:uid="{9D4B1E4E-0BB2-4C06-BDCC-4A361BC1C401}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -29196,21 +29195,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29454,19 +29453,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D95885E-3D3E-41C7-BCB5-60294B0AB1EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C49041-F246-4B03-A83A-30F6FFFE0FD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D95885E-3D3E-41C7-BCB5-60294B0AB1EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>